<commit_message>
TC values need to be rounded, Excel summary pahe needs update
</commit_message>
<xml_diff>
--- a/QTO_Tool/Resources/Excel/template.xlsx
+++ b/QTO_Tool/Resources/Excel/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anaderpour\OneDrive - Turner Construction\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anaderpour\OneDrive - Turner Construction\Documents\Project\Rhino\QTO_Tool\QTO_Tool\Resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A62E274-79A8-4E82-9A13-1763E1B5DD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D7FDF7-13D1-43EA-B7A3-0EA65701C673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>N/A</t>
   </si>
@@ -128,7 +128,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +147,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,7 +225,44 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="28">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9ACD32"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -283,85 +326,6 @@
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9ACD32"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -376,53 +340,53 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:P2" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:P2" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:P2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="16">
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COUNT" dataDxfId="15">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="COUNT" dataDxfId="25">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!F$2:F$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="NAME ABB." dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="GROSS VOLUME" dataDxfId="13" dataCellStyle="Comma">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="NAME ABB." dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="GROSS VOLUME" dataDxfId="23" dataCellStyle="Comma">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!I$2:I$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="NET VOLUME" dataDxfId="12">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="NET VOLUME" dataDxfId="22">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!J$2:J$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="BOTTOM AREA" dataDxfId="11">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="BOTTOM AREA" dataDxfId="21">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!K$2:K$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="OPENING AREA" dataDxfId="10">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="OPENING AREA" dataDxfId="20">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!L$2:L$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="TOP AREA" dataDxfId="9">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="TOP AREA" dataDxfId="19">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!M$2:M$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SIDE AREA" dataDxfId="8">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SIDE AREA" dataDxfId="18">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!N$2:N$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="END AREA" dataDxfId="7">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="END AREA" dataDxfId="17">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!O$2:O$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="SIDE-1" dataDxfId="6">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="SIDE-1" dataDxfId="16">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!P$2:P$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="SIDE-2" dataDxfId="5">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="SIDE-2" dataDxfId="15">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!Q$2:Q$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="EDGE AREA" dataDxfId="4">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="EDGE AREA" dataDxfId="14">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!R$2:R$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="LENGTH" dataDxfId="3">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="LENGTH" dataDxfId="13">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!S$2:S$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="HEIGHT" dataDxfId="2">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="HEIGHT" dataDxfId="12">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!T$2:T$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="PERIMETER" dataDxfId="1">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="PERIMETER" dataDxfId="11">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!U$2:U$199)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="OPENING PERIMETER" dataDxfId="0">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="OPENING PERIMETER" dataDxfId="10">
       <calculatedColumnFormula>SUMIF(PROJECT!$G$2:$G$199,$B2,PROJECT!V$2:V$199)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -431,33 +395,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:V2" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="A1:V2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="C1" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="C2" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="C3" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="C4" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="C5" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="COUNT" dataDxfId="34"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="NAME ABB." dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:H2" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="C1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="C2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="C3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="C4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="C5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="COUNT" dataDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="NAME ABB." dataDxfId="1">
       <calculatedColumnFormula>A2&amp;" "&amp;B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="NAME" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="GROSS VOLUME" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="NET VOLUME" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="BOTTOM AREA" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="OPENING AREA" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="TOP AREA" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="SIDE AREA" dataDxfId="26"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="END AREA" dataDxfId="25"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="SIDE-1" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="SIDE-2" dataDxfId="23"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="EDGE AREA" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="LENGTH" dataDxfId="21"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="HEIGHT" dataDxfId="20"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="PERIMETER" dataDxfId="19"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="OPENING PERIMETER" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="NAME" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1387,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V199"/>
+  <dimension ref="A1:W199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1418,7 +1368,7 @@
     <col min="22" max="22" width="21.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1443,50 +1393,23 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -1512,50 +1435,22 @@
       <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2">
-        <v>0</v>
-      </c>
-      <c r="U2" s="2">
-        <v>0</v>
-      </c>
-      <c r="V2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1579,7 +1474,7 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1603,7 +1498,7 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1627,7 +1522,7 @@
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1651,7 +1546,7 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1675,7 +1570,7 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1699,7 +1594,7 @@
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1723,7 +1618,7 @@
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1747,7 +1642,7 @@
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1771,7 +1666,7 @@
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1795,7 +1690,7 @@
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1819,7 +1714,7 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1843,7 +1738,7 @@
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1867,7 +1762,7 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -6221,6 +6116,7 @@
       <c r="G199" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Elevation Input has been fully incorporated
</commit_message>
<xml_diff>
--- a/QTO_Tool/Resources/Excel/template.xlsx
+++ b/QTO_Tool/Resources/Excel/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anaderpour\OneDrive - Turner Construction\Documents\Project\Rhino\QTO_Tool\QTO_Tool\Resources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PersonalProjects\Rhino\QTO_Tool\QTO_Tool\Resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C2F9DA-CBC7-44F9-9754-BCFD22AEB537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5486F9DA-A54E-4EC0-9A29-9EA4A2222180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-76910" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,6 +183,40 @@
   </cellStyles>
   <dxfs count="24">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9ACD32"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -239,40 +273,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9ACD32"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -367,23 +367,23 @@
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="SIDE-1" dataDxfId="12"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="SIDE-2" dataDxfId="11"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="EDGE AREA" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{549CC8E3-D79D-4F7B-9730-EE177BA1EBF0}" name="TREAD AREA" dataDxfId="0" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{DB428909-2267-4D8A-9CB9-17B792CEE33C}" name="RISER AREA" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="2" xr3:uid="{A187C0EE-0AA0-4BF7-B0C9-D88BADD855FB}" name="TREAD COUNT" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="LENGTH" dataDxfId="9"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="HEIGHT" dataDxfId="8"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="PERIMETER" dataDxfId="7"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="OPENING PERIMETER" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{549CC8E3-D79D-4F7B-9730-EE177BA1EBF0}" name="TREAD AREA" dataDxfId="9" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{DB428909-2267-4D8A-9CB9-17B792CEE33C}" name="RISER AREA" dataDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{A187C0EE-0AA0-4BF7-B0C9-D88BADD855FB}" name="TREAD COUNT" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="LENGTH" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="HEIGHT" dataDxfId="5"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="PERIMETER" dataDxfId="4"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="OPENING PERIMETER" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="PROJECT_TABLE" displayName="PROJECT_TABLE" ref="A1:A2" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="PROJECT_TABLE" displayName="PROJECT_TABLE" ref="A1:A2" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="A1:A2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="NAME" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="NAME" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -689,7 +689,7 @@
   <dimension ref="A1:S196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1256,7 +1256,7 @@
   <dimension ref="A1:P196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>